<commit_message>
Test data for TC-147 is updated and updated test script for 1826 user story
</commit_message>
<xml_diff>
--- a/Test Data/TC_147_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_RBus_Connection.xlsx
+++ b/Test Data/TC_147_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_RBus_Connection.xlsx
@@ -1,32 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhasip\Desktop\NGConsys Automation_01_02_2019\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA31EF7-3657-42A1-8184-E85C6A15BFFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Color Codes</t>
   </si>
@@ -152,12 +158,27 @@
   </si>
   <si>
     <t>Default Alarm Load</t>
+  </si>
+  <si>
+    <t>Total Battery Standby</t>
+  </si>
+  <si>
+    <t>Total Alarm Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Battery Standby after Deleting device</t>
+  </si>
+  <si>
+    <t>Alarm Load after Deleting device</t>
+  </si>
+  <si>
+    <t>Battery and Alarm Load Values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +312,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -298,6 +325,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -579,11 +609,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,33 +636,33 @@
     <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -647,7 +677,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -660,7 +690,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
       <c r="D5" s="8" t="s">
         <v>7</v>
@@ -669,24 +699,30 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
       <c r="M6" s="17"/>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
       <c r="R6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+    </row>
+    <row r="7" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -738,8 +774,20 @@
       <c r="R7" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -756,10 +804,10 @@
         <v>14</v>
       </c>
       <c r="F8" s="16">
-        <v>0.30099999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="G8" s="16">
-        <v>0.38700000000000001</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>28</v>
@@ -791,20 +839,34 @@
       <c r="R8" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
+      <c r="S8" s="19">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="T8" s="19">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="U8" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="V8" s="19">
+        <v>0.61199999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="S6:V6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated test data for FC test cases
</commit_message>
<xml_diff>
--- a/Test Data/TC_147_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_RBus_Connection.xlsx
+++ b/Test Data/TC_147_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_RBus_Connection.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Color Codes</t>
   </si>
@@ -286,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -328,6 +328,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -624,7 +627,7 @@
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8:X8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,7 +637,7 @@
     <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
@@ -649,15 +652,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -666,15 +673,19 @@
       <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -713,26 +724,26 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
       <c r="M6" s="17"/>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
       <c r="R6" s="17"/>
-      <c r="S6" s="23" t="s">
+      <c r="S6" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
     </row>
     <row r="7" spans="1:24" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">

</xml_diff>